<commit_message>
Added MCU and LoRa module PCB's components in BOM
</commit_message>
<xml_diff>
--- a/src/bom.xlsx
+++ b/src/bom.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cools\code\iot19-md2\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80B3261D-CA94-487B-B053-22AD2F015068}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{376BAF66-BE59-4E12-BBFE-BB7CFFEC3127}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2355" yWindow="-16320" windowWidth="29040" windowHeight="15990" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2355" yWindow="-16320" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Handleiding" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="113">
   <si>
     <t>Hoe gebruik je deze excelsheet</t>
   </si>
@@ -162,13 +162,214 @@
   </si>
   <si>
     <t>https://be.farnell.com/microchip/mic5219-3-3ym5-tr/ldo-0-5vdo-0-5a-3-3v-1-5sot23/dp/2510252?st=MIC5219-3.3YM5-TR</t>
+  </si>
+  <si>
+    <t>Y1</t>
+  </si>
+  <si>
+    <t>https://be.farnell.com/abracon/abs07-32-768khz-t/crystal-32-768khz-12-5pf-smd/dp/2101347?scope=partnumberlookahead&amp;ost=2101347&amp;searchref=searchlookahead&amp;exaMfpn=true&amp;ddkey=https%3Anl-BE%2FElement14_Belgium%2Fw%2Fsearch</t>
+  </si>
+  <si>
+    <t>32.768 kHz crystal</t>
+  </si>
+  <si>
+    <t>ABRACON</t>
+  </si>
+  <si>
+    <t>ABS07-32.768KHZ-T</t>
+  </si>
+  <si>
+    <t>SMD</t>
+  </si>
+  <si>
+    <t>C1, C2</t>
+  </si>
+  <si>
+    <t>https://be.farnell.com/kemet/c0805c150j5gactu/cap-15pf-50v-5-c0g-np0-0805/dp/1414668?st=capacitor%200805%2015%20pF</t>
+  </si>
+  <si>
+    <t>15 pF Capacitors</t>
+  </si>
+  <si>
+    <t>C0805C150J5GACTU</t>
+  </si>
+  <si>
+    <t>KEMET</t>
+  </si>
+  <si>
+    <t>IC1</t>
+  </si>
+  <si>
+    <t>MICROCHIP</t>
+  </si>
+  <si>
+    <t>SOT-23-5</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>2.2uF Capacitor</t>
+  </si>
+  <si>
+    <t>TAIYO YUDEN</t>
+  </si>
+  <si>
+    <t>UMK212BB7225KG-T</t>
+  </si>
+  <si>
+    <t>https://be.farnell.com/taiyo-yuden/umk212bb7225kg-t/capacitor-mlcc-x7r-2-2uf-50v-0805/dp/2779058?st=capacitor%200805%202.2uF</t>
+  </si>
+  <si>
+    <t>SMD 0805</t>
+  </si>
+  <si>
+    <t>C4</t>
+  </si>
+  <si>
+    <t>470pF Capacitor</t>
+  </si>
+  <si>
+    <t>MULTICOMP</t>
+  </si>
+  <si>
+    <t>MC0805B471M101CT</t>
+  </si>
+  <si>
+    <t>https://be.farnell.com/multicomp/mc0805b471m101ct/ceramic-capacitor-470pf-100v-x7r/dp/1708840?st=capacitor%200805%20470pF</t>
+  </si>
+  <si>
+    <t>10kOhm resistor</t>
+  </si>
+  <si>
+    <t>VISHAY</t>
+  </si>
+  <si>
+    <t>CRCW080510K0FKEA</t>
+  </si>
+  <si>
+    <t>1469856RL</t>
+  </si>
+  <si>
+    <t>https://be.farnell.com/vishay/crcw080510k0fkea/res-10k-1-0-125w-0805-thick-film/dp/1469856RL?st=0805%2010k%20ohm</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>330Ohm resistor</t>
+  </si>
+  <si>
+    <t>https://be.farnell.com/vishay/crcw0805330rfkea/res-330r-1-0-125w-0805-thick-film/dp/1469918?st=0805%2010k%20ohm</t>
+  </si>
+  <si>
+    <t>CRCW0805330RFKEA</t>
+  </si>
+  <si>
+    <t>https://be.farnell.com/avx/08051c104jat2a/cap-0-1-f-100v-5-x7r-0805/dp/2332715RL?st=0805%20100nF</t>
+  </si>
+  <si>
+    <t>2332715RL</t>
+  </si>
+  <si>
+    <t>08051C104JAT2A</t>
+  </si>
+  <si>
+    <t>AVX</t>
+  </si>
+  <si>
+    <t>C6, C5</t>
+  </si>
+  <si>
+    <t>100 nF capacitor/ 0.1uF</t>
+  </si>
+  <si>
+    <t>https://be.farnell.com/avx/08053c105k4z2a/cap-1-f-25v-10-x7r-0805/dp/1833845?st=0805%201uF</t>
+  </si>
+  <si>
+    <t>08053C105K4Z2A</t>
+  </si>
+  <si>
+    <t>1 uF capacitor</t>
+  </si>
+  <si>
+    <t>C7</t>
+  </si>
+  <si>
+    <t>SMD switch</t>
+  </si>
+  <si>
+    <t>S1</t>
+  </si>
+  <si>
+    <t>https://be.farnell.com/omron/b3fs-1000/tactile-switch-0-05a-24vdc-illum/dp/3121161?st=smd%20switch</t>
+  </si>
+  <si>
+    <t>B3FS-1000</t>
+  </si>
+  <si>
+    <t>OMRON</t>
+  </si>
+  <si>
+    <t>ATSAMD21G18A-AU</t>
+  </si>
+  <si>
+    <t>IC2</t>
+  </si>
+  <si>
+    <t>48-pin TQFP</t>
+  </si>
+  <si>
+    <t>https://be.farnell.com/microchip/atsamd21g18a-au/mcu-32bit-cortex-m0-48mhz-tqfp/dp/2409248?st=ATSAMD21G</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>10 uF capacitor</t>
+  </si>
+  <si>
+    <t>https://be.farnell.com/avx/08053d106kat2a/cap-10-f-25v-10-x5r-0805/dp/1867958?st=0805%2010uF</t>
+  </si>
+  <si>
+    <t>08053D106KAT2A</t>
+  </si>
+  <si>
+    <t>LORAMODULE</t>
+  </si>
+  <si>
+    <t>RFM95W-868S2</t>
+  </si>
+  <si>
+    <t>HOPERF</t>
+  </si>
+  <si>
+    <t>https://be.farnell.com/hoperf/rfm95w-868s2/transceiver-868mhz-fsk-ook/dp/2759294?st=RFm95W</t>
+  </si>
+  <si>
+    <t>J1</t>
+  </si>
+  <si>
+    <t>Antenna pin</t>
+  </si>
+  <si>
+    <t>https://be.farnell.com/hirose-hrs/u-fl-r-smt-01/rf-coaxial-u-fl-straight-jack/dp/3908021?ost=U.FL-R-SMT(01)&amp;ddkey=https%3Anl-BE%2FElement14_Belgium%2Fsearch</t>
+  </si>
+  <si>
+    <t>U.FL-R-SMT(01)</t>
+  </si>
+  <si>
+    <t>HIROSE(HRS)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -220,6 +421,29 @@
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -259,10 +483,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -283,14 +508,19 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -509,7 +739,9 @@
   </sheetPr>
   <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K22" sqref="K22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -518,33 +750,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="3:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
     </row>
     <row r="2" spans="3:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
+      <c r="C2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
     </row>
     <row r="3" spans="3:8" ht="13" x14ac:dyDescent="0.3">
       <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="15" t="s">
+      <c r="E3" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
     </row>
     <row r="4" spans="3:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4" s="6" t="s">
@@ -553,12 +785,12 @@
       <c r="D4" s="5">
         <v>1</v>
       </c>
-      <c r="E4" s="12" t="s">
+      <c r="E4" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
     </row>
     <row r="5" spans="3:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C5" s="5" t="s">
@@ -567,12 +799,12 @@
       <c r="D5" s="5">
         <v>2</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="E5" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
     </row>
     <row r="6" spans="3:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" s="5" t="s">
@@ -581,12 +813,12 @@
       <c r="D6" s="5">
         <v>3</v>
       </c>
-      <c r="E6" s="12" t="s">
+      <c r="E6" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="13"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
     </row>
     <row r="7" spans="3:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C7" s="6" t="s">
@@ -595,12 +827,12 @@
       <c r="D7" s="5">
         <v>4</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c r="E7" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
     </row>
     <row r="8" spans="3:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C8" s="5" t="s">
@@ -609,30 +841,30 @@
       <c r="D8" s="5">
         <v>5</v>
       </c>
-      <c r="E8" s="12" t="s">
+      <c r="E8" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="13"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
     </row>
     <row r="9" spans="3:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C9" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="13"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="14"/>
     </row>
     <row r="10" spans="3:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C10" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
     </row>
     <row r="11" spans="3:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C11" s="5" t="s">
@@ -710,7 +942,7 @@
       <c r="J20" s="5">
         <v>1128068</v>
       </c>
-      <c r="K20" s="8" t="s">
+      <c r="K20" s="17" t="s">
         <v>36</v>
       </c>
     </row>
@@ -744,7 +976,7 @@
       <c r="B22" s="5">
         <v>1</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="C22" s="19" t="s">
         <v>41</v>
       </c>
       <c r="D22" s="6" t="s">
@@ -803,10 +1035,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AE1"/>
+  <dimension ref="A1:AE12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:J1"/>
+      <selection activeCell="B9" sqref="B9:J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -814,10 +1046,11 @@
     <col min="1" max="1" width="21.81640625" customWidth="1"/>
     <col min="2" max="2" width="14.453125" customWidth="1"/>
     <col min="3" max="3" width="72.54296875" customWidth="1"/>
+    <col min="7" max="7" width="22.1796875" customWidth="1"/>
     <col min="9" max="9" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -870,8 +1103,377 @@
       <c r="AD1" s="4"/>
       <c r="AE1" s="4"/>
     </row>
+    <row r="2" spans="1:31" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="12">
+        <v>1</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="E2" s="12">
+        <v>0.745</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="I2" s="12">
+        <v>2101347</v>
+      </c>
+      <c r="J2" s="17" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" s="12">
+        <v>2</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="E3" s="12">
+        <v>6.83E-2</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="I3" s="12">
+        <v>1414668</v>
+      </c>
+      <c r="J3" s="17" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" s="12">
+        <v>1</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E4" s="12">
+        <v>0.80800000000000005</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="H4" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="I4" s="12">
+        <v>2510252</v>
+      </c>
+      <c r="J4" s="17" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="B5" s="12">
+        <v>1</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="E5" s="12">
+        <v>0.28100000000000003</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="I5" s="12">
+        <v>2779058</v>
+      </c>
+      <c r="J5" s="17" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="B6" s="12">
+        <v>2</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="E6" s="12">
+        <v>6.1699999999999998E-2</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="H6" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="I6" s="12">
+        <v>1708840</v>
+      </c>
+      <c r="J6" s="17" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="12">
+        <v>1</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="E7" s="12">
+        <v>2.7199999999999998E-2</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="H7" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="I7" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="J7" s="17" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="B8" s="12">
+        <v>1</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="E8" s="12">
+        <v>3.0800000000000001E-2</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="H8" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="I8" s="12">
+        <v>1469918</v>
+      </c>
+      <c r="J8" s="17" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="9" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="B9" s="12">
+        <v>1</v>
+      </c>
+      <c r="C9" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="E9" s="12">
+        <v>0.28100000000000003</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="H9" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="I9" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="J9" s="17" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="B10" s="12">
+        <v>1</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="E10" s="12">
+        <v>0.36</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="G10" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="H10" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="I10" s="12">
+        <v>1833845</v>
+      </c>
+      <c r="J10" s="17" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="11" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="B11" s="12">
+        <v>1</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="E11" s="12">
+        <v>0.41099999999999998</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="G11" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="H11" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="I11" s="12">
+        <v>3121161</v>
+      </c>
+      <c r="J11" s="17" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="12" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="B12" s="12">
+        <v>1</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="E12" s="12">
+        <v>2.79</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="G12" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="H12" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="I12" s="12">
+        <v>2409248</v>
+      </c>
+      <c r="J12" s="17" t="s">
+        <v>98</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="13" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="J2" r:id="rId1" xr:uid="{630D719B-C5E5-46AF-9E34-0A2B57A36183}"/>
+    <hyperlink ref="J3" r:id="rId2" xr:uid="{43906569-DE1F-494D-B842-A4D1BC0D7402}"/>
+    <hyperlink ref="J4" r:id="rId3" xr:uid="{8D2A9D91-8760-4462-B06E-959D9DB2284C}"/>
+    <hyperlink ref="J5" r:id="rId4" xr:uid="{C6CD174E-DD66-43C3-8DC9-E3E6C2487E35}"/>
+    <hyperlink ref="J6" r:id="rId5" xr:uid="{11D06CE2-A300-4393-9B4A-29C214982943}"/>
+    <hyperlink ref="F7" r:id="rId6" display="https://be.farnell.com/b/vishay" xr:uid="{313380DD-4C4E-4FE3-895A-9B5666D6B1D3}"/>
+    <hyperlink ref="J7" r:id="rId7" xr:uid="{362F830D-7D9F-4C6B-84B0-69265E426E5B}"/>
+    <hyperlink ref="J8" r:id="rId8" xr:uid="{E7907A67-F98B-4353-B3D2-E3194CE5B42A}"/>
+    <hyperlink ref="F8" r:id="rId9" display="https://be.farnell.com/b/vishay" xr:uid="{22204F88-2837-45F3-84CB-720F22A267F8}"/>
+    <hyperlink ref="J9" r:id="rId10" xr:uid="{593DFB5D-51A1-4079-9FF4-F0A343BCB055}"/>
+    <hyperlink ref="J10" r:id="rId11" xr:uid="{2558B278-230E-4382-B4FE-5D4ED8A1B889}"/>
+    <hyperlink ref="J11" r:id="rId12" xr:uid="{F56A9E07-452D-4EFD-AA58-29A5BDFA06E7}"/>
+    <hyperlink ref="J12" r:id="rId13" xr:uid="{CE1AA630-4ECF-4248-8D2C-AABDA0D6A677}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId14"/>
 </worksheet>
 </file>
 
@@ -880,16 +1482,18 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AE1"/>
+  <dimension ref="A1:AE6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:J1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.81640625" customWidth="1"/>
-    <col min="2" max="3" width="72.54296875" customWidth="1"/>
+    <col min="2" max="2" width="9.08984375" customWidth="1"/>
+    <col min="3" max="3" width="51.36328125" customWidth="1"/>
+    <col min="7" max="7" width="16.90625" customWidth="1"/>
     <col min="9" max="9" width="16" customWidth="1"/>
   </cols>
   <sheetData>
@@ -946,7 +1550,173 @@
       <c r="AD1" s="7"/>
       <c r="AE1" s="7"/>
     </row>
+    <row r="2" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" s="12">
+        <v>1</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="E2" s="12">
+        <v>0.28100000000000003</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="I2" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="J2" s="17" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="B3" s="12">
+        <v>1</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="E3" s="12">
+        <v>0.36</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="I3" s="12">
+        <v>1833845</v>
+      </c>
+      <c r="J3" s="17" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="B4" s="18">
+        <v>1</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="E4" s="18">
+        <v>0.59</v>
+      </c>
+      <c r="F4" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="G4" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="H4" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="I4" s="18">
+        <v>1867958</v>
+      </c>
+      <c r="J4" s="17" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="5" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="18" t="s">
+        <v>104</v>
+      </c>
+      <c r="B5" s="18">
+        <v>1</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="E5" s="18">
+        <v>22.73</v>
+      </c>
+      <c r="F5" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="G5" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="H5" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="I5" s="18">
+        <v>2759294</v>
+      </c>
+      <c r="J5" s="17" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="6" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="B6" s="18">
+        <v>1</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18">
+        <v>0.97</v>
+      </c>
+      <c r="F6" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="G6" s="18" t="s">
+        <v>111</v>
+      </c>
+      <c r="H6" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="I6" s="18">
+        <v>3908021</v>
+      </c>
+      <c r="J6" s="17" t="s">
+        <v>110</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="13" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="J2" r:id="rId1" xr:uid="{188B0C9C-89EA-47AB-9AA3-0A633F1B92E3}"/>
+    <hyperlink ref="J3" r:id="rId2" xr:uid="{87E6912A-FB9A-40D9-A77F-498E8330FD6F}"/>
+    <hyperlink ref="J4" r:id="rId3" xr:uid="{AC7311C6-BCD5-4778-914E-DB9DF8EE629E}"/>
+    <hyperlink ref="J5" r:id="rId4" xr:uid="{409C9877-FD72-4B2B-B1A3-E8280432C0DF}"/>
+    <hyperlink ref="J6" r:id="rId5" xr:uid="{2F4D3A20-EE95-4193-A4D6-EF48AAF522F5}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -972,7 +1742,7 @@
     <col min="10" max="10" width="22.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="62.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="31.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>3</v>
       </c>
@@ -1014,7 +1784,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66F0071E-D3A6-4DED-AB23-7E39BD16B86A}">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:J1"/>
     </sheetView>
   </sheetViews>
@@ -1032,7 +1802,7 @@
     <col min="10" max="10" width="19.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="62.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="31.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
bom gps and humidity
</commit_message>
<xml_diff>
--- a/src/bom.xlsx
+++ b/src/bom.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cools\code\iot19-md2\src\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Imad\Documents\3dejaar\IoT\Medical_Delivery_Box_proj\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80B3261D-CA94-487B-B053-22AD2F015068}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B03A8781-AC5D-4D88-A116-5E3447690BD6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2355" yWindow="-16320" windowWidth="29040" windowHeight="15990" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12576" yWindow="1092" windowWidth="17280" windowHeight="8964" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Handleiding" sheetId="1" r:id="rId1"/>
@@ -19,12 +19,20 @@
     <sheet name="PCB GPS module" sheetId="4" r:id="rId4"/>
     <sheet name="PCB HumidityTemp module" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="91">
   <si>
     <t>Hoe gebruik je deze excelsheet</t>
   </si>
@@ -162,13 +170,151 @@
   </si>
   <si>
     <t>https://be.farnell.com/microchip/mic5219-3-3ym5-tr/ldo-0-5vdo-0-5a-3-3v-1-5sot23/dp/2510252?st=MIC5219-3.3YM5-TR</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>U.FL</t>
+  </si>
+  <si>
+    <t>100 Ω weerstand</t>
+  </si>
+  <si>
+    <t>120 Ω weerstand</t>
+  </si>
+  <si>
+    <t>27pF capacitor</t>
+  </si>
+  <si>
+    <t>Male U.FL connector (antenna)</t>
+  </si>
+  <si>
+    <t>SMD</t>
+  </si>
+  <si>
+    <t>PANASONIC</t>
+  </si>
+  <si>
+    <t>WALSIN</t>
+  </si>
+  <si>
+    <t>HIROSE(HRS)</t>
+  </si>
+  <si>
+    <t>ERJP06F1200V</t>
+  </si>
+  <si>
+    <t>0805N270J500CT</t>
+  </si>
+  <si>
+    <t>U.FL-R-SMT(01)</t>
+  </si>
+  <si>
+    <t>ERJP06F1000V</t>
+  </si>
+  <si>
+    <t>https://nl.farnell.com/panasonic/erjp06f1000v/res-100r-1-0-5w-0805-thick-film/dp/1750741?st=ERJP06%20Series</t>
+  </si>
+  <si>
+    <t>https://be.farnell.com/panasonic/erjp06f1200v/res-120r-1-0-5w-0805-thick-film/dp/1750742</t>
+  </si>
+  <si>
+    <t>https://be.farnell.com/walsin/0805n270j500ct/cap-27pf-50v-5-c0g-np0-0805-reel/dp/2495527</t>
+  </si>
+  <si>
+    <t>https://be.farnell.com/hirose-hrs/u-fl-r-smt-01/rf-coaxial-u-fl-straight-jack/dp/3908021?ost=U.FL-R-SMT%2801%29&amp;ddkey=https%3Anl-BE%2FElement14_Belgium%2Fsearch</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>C4</t>
+  </si>
+  <si>
+    <t>10µF capacitor</t>
+  </si>
+  <si>
+    <t>100nF capacitor</t>
+  </si>
+  <si>
+    <t>1µF capacitor</t>
+  </si>
+  <si>
+    <t>AVX</t>
+  </si>
+  <si>
+    <t>0805ZC106KAT2A</t>
+  </si>
+  <si>
+    <t>2094042RL</t>
+  </si>
+  <si>
+    <t>08051C104K4T2A</t>
+  </si>
+  <si>
+    <t>08053C105KAT2A</t>
+  </si>
+  <si>
+    <t>https://be.farnell.com/avx/0805zc106kat2a/cap-mlcc-x7r-10uf-10v-0805/dp/2094042RL</t>
+  </si>
+  <si>
+    <t>https://be.farnell.com/avx/08051c104k4t2a/cap-0-1-f-100v-10-x7r-0805/dp/1833888?st=100nf%20smd%200805</t>
+  </si>
+  <si>
+    <t>https://be.farnell.com/avx/08053c105kat2a/cap-1-f-25v-10-x7r-0805/dp/1658877?st=1%C2%B5f%20smd%200805</t>
+  </si>
+  <si>
+    <t>HIH6030-021-001</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>0.22µF capacitor</t>
+  </si>
+  <si>
+    <t>0.1µF capacitor</t>
+  </si>
+  <si>
+    <t>2.2k resistors</t>
+  </si>
+  <si>
+    <t>Humidity sensor</t>
+  </si>
+  <si>
+    <t>HONEYWELL</t>
+  </si>
+  <si>
+    <t>ERA6AEB222V</t>
+  </si>
+  <si>
+    <t>08055C224KAT2A</t>
+  </si>
+  <si>
+    <t>https://be.farnell.com/avx/08055c224kat2a/cap-0-22-f-50v-10-x7r-0805/dp/1658878?st=0.22%C2%B5F%20smd</t>
+  </si>
+  <si>
+    <t>https://be.farnell.com/panasonic/era6aeb222v/res-2k2-0-1-0-125w-0805-thin-film/dp/1577663?st=2.2k%20resistors%20smd</t>
+  </si>
+  <si>
+    <t>https://be.farnell.com/honeywell-s-c/hih-6030-021-001/sensor-humidity-no-filter-4-5-8soic/dp/2356755</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="[$€-2]\ #,##0.00;[Red]\-[$€-2]\ #,##0.00"/>
+  </numFmts>
+  <fonts count="12">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -220,6 +366,18 @@
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -259,10 +417,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -283,14 +442,23 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -511,140 +679,140 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="3" max="3" width="72.81640625" customWidth="1"/>
+    <col min="3" max="3" width="72.77734375" customWidth="1"/>
     <col min="8" max="8" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C1" s="14" t="s">
+    <row r="1" spans="3:8" ht="15.75" customHeight="1">
+      <c r="C1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-    </row>
-    <row r="2" spans="3:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-    </row>
-    <row r="3" spans="3:8" ht="13" x14ac:dyDescent="0.3">
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+    </row>
+    <row r="2" spans="3:8" ht="15.75" customHeight="1">
+      <c r="C2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+    </row>
+    <row r="3" spans="3:8" ht="13.2">
       <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="15" t="s">
+      <c r="E3" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-    </row>
-    <row r="4" spans="3:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+    </row>
+    <row r="4" spans="3:8" ht="15.75" customHeight="1">
       <c r="C4" s="6" t="s">
         <v>14</v>
       </c>
       <c r="D4" s="5">
         <v>1</v>
       </c>
-      <c r="E4" s="12" t="s">
+      <c r="E4" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
-    </row>
-    <row r="5" spans="3:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+    </row>
+    <row r="5" spans="3:8" ht="15.75" customHeight="1">
       <c r="C5" s="5" t="s">
         <v>16</v>
       </c>
       <c r="D5" s="5">
         <v>2</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="E5" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
-    </row>
-    <row r="6" spans="3:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+    </row>
+    <row r="6" spans="3:8" ht="15.75" customHeight="1">
       <c r="C6" s="5" t="s">
         <v>18</v>
       </c>
       <c r="D6" s="5">
         <v>3</v>
       </c>
-      <c r="E6" s="12" t="s">
+      <c r="E6" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="13"/>
-    </row>
-    <row r="7" spans="3:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+    </row>
+    <row r="7" spans="3:8" ht="15.75" customHeight="1">
       <c r="C7" s="6" t="s">
         <v>20</v>
       </c>
       <c r="D7" s="5">
         <v>4</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c r="E7" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13"/>
-    </row>
-    <row r="8" spans="3:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+    </row>
+    <row r="8" spans="3:8" ht="15.75" customHeight="1">
       <c r="C8" s="5" t="s">
         <v>22</v>
       </c>
       <c r="D8" s="5">
         <v>5</v>
       </c>
-      <c r="E8" s="12" t="s">
+      <c r="E8" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="13"/>
-    </row>
-    <row r="9" spans="3:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+    </row>
+    <row r="9" spans="3:8" ht="15.75" customHeight="1">
       <c r="C9" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="13"/>
-    </row>
-    <row r="10" spans="3:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="14"/>
+    </row>
+    <row r="10" spans="3:8" ht="15.75" customHeight="1">
       <c r="C10" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
-    </row>
-    <row r="11" spans="3:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
+    </row>
+    <row r="11" spans="3:8" ht="15.75" customHeight="1">
       <c r="C11" s="5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="3:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:8" ht="15.75" customHeight="1">
       <c r="C12" s="6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" ht="15.75" customHeight="1">
       <c r="A19" s="3" t="s">
         <v>3</v>
       </c>
@@ -679,7 +847,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" ht="15.75" customHeight="1">
       <c r="A20" s="5" t="s">
         <v>29</v>
       </c>
@@ -714,7 +882,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" ht="15.75" customHeight="1">
       <c r="A21" s="10" t="s">
         <v>37</v>
       </c>
@@ -737,7 +905,7 @@
       <c r="J21" s="11"/>
       <c r="K21" s="11"/>
     </row>
-    <row r="22" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" ht="15.75" customHeight="1">
       <c r="A22" s="6" t="s">
         <v>37</v>
       </c>
@@ -809,15 +977,15 @@
       <selection sqref="A1:J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="21.81640625" customWidth="1"/>
-    <col min="2" max="2" width="14.453125" customWidth="1"/>
-    <col min="3" max="3" width="72.54296875" customWidth="1"/>
+    <col min="1" max="1" width="21.77734375" customWidth="1"/>
+    <col min="2" max="2" width="14.44140625" customWidth="1"/>
+    <col min="3" max="3" width="72.5546875" customWidth="1"/>
     <col min="9" max="9" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" ht="37.5" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -886,14 +1054,14 @@
       <selection sqref="A1:J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="21.81640625" customWidth="1"/>
-    <col min="2" max="3" width="72.54296875" customWidth="1"/>
+    <col min="1" max="1" width="21.77734375" customWidth="1"/>
+    <col min="2" max="3" width="72.5546875" customWidth="1"/>
     <col min="9" max="9" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" ht="37.5" customHeight="1">
       <c r="A1" s="3" t="s">
         <v>3</v>
       </c>
@@ -953,26 +1121,26 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56C8A83F-0A92-42E1-85C1-9A9ADB6E359F}">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:J1"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.2"/>
   <cols>
-    <col min="1" max="1" width="22.7265625" customWidth="1"/>
-    <col min="3" max="3" width="33.7265625" customWidth="1"/>
-    <col min="4" max="4" width="25.6328125" customWidth="1"/>
-    <col min="5" max="5" width="19.36328125" customWidth="1"/>
-    <col min="6" max="6" width="14.08984375" customWidth="1"/>
-    <col min="7" max="7" width="21.1796875" customWidth="1"/>
-    <col min="8" max="8" width="19.81640625" customWidth="1"/>
-    <col min="9" max="9" width="21.81640625" customWidth="1"/>
-    <col min="10" max="10" width="22.1796875" customWidth="1"/>
+    <col min="1" max="1" width="22.77734375" customWidth="1"/>
+    <col min="3" max="3" width="33.77734375" customWidth="1"/>
+    <col min="4" max="4" width="25.6640625" customWidth="1"/>
+    <col min="5" max="5" width="19.33203125" customWidth="1"/>
+    <col min="6" max="6" width="15.5546875" customWidth="1"/>
+    <col min="7" max="7" width="21.21875" customWidth="1"/>
+    <col min="8" max="8" width="19.77734375" customWidth="1"/>
+    <col min="9" max="9" width="21.77734375" customWidth="1"/>
+    <col min="10" max="10" width="22.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="62.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="16.2" thickBot="1">
       <c r="A1" s="3" t="s">
         <v>3</v>
       </c>
@@ -1004,35 +1172,268 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="13" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:10" ht="13.8" thickTop="1">
+      <c r="A2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E2" s="17">
+        <v>5.5999999999999999E-3</v>
+      </c>
+      <c r="F2" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="G2" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="H2" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="I2">
+        <v>1750741</v>
+      </c>
+      <c r="J2" s="18" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E3" s="17">
+        <v>9.8299999999999998E-2</v>
+      </c>
+      <c r="F3" t="s">
+        <v>54</v>
+      </c>
+      <c r="G3" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="H3" t="s">
+        <v>35</v>
+      </c>
+      <c r="I3">
+        <v>1750742</v>
+      </c>
+      <c r="J3" s="18" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E4" s="17">
+        <v>1.1900000000000001E-2</v>
+      </c>
+      <c r="F4" t="s">
+        <v>55</v>
+      </c>
+      <c r="G4" t="s">
+        <v>58</v>
+      </c>
+      <c r="H4" t="s">
+        <v>35</v>
+      </c>
+      <c r="I4">
+        <v>2495527</v>
+      </c>
+      <c r="J4" s="18" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E5" s="17">
+        <v>0.97</v>
+      </c>
+      <c r="F5" t="s">
+        <v>56</v>
+      </c>
+      <c r="G5" t="s">
+        <v>59</v>
+      </c>
+      <c r="H5" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="I5">
+        <v>3908021</v>
+      </c>
+      <c r="J5" s="18" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="D6" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="E6" s="17">
+        <v>0.88400000000000001</v>
+      </c>
+      <c r="F6" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="G6" t="s">
+        <v>72</v>
+      </c>
+      <c r="H6" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="I6" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="J6" s="18" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="E7" s="20">
+        <v>0.316</v>
+      </c>
+      <c r="F7" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="G7" t="s">
+        <v>74</v>
+      </c>
+      <c r="H7" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="I7">
+        <v>1833888</v>
+      </c>
+      <c r="J7" s="18" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" s="12" customFormat="1">
+      <c r="A8" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="B8" s="12">
+        <v>1</v>
+      </c>
+      <c r="C8" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="E8" s="17">
+        <v>0.20200000000000001</v>
+      </c>
+      <c r="F8" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="H8" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="I8" s="12">
+        <v>1658877</v>
+      </c>
+      <c r="J8" s="18" t="s">
+        <v>78</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="J2" r:id="rId1" xr:uid="{8BBE50AA-998B-4F4E-AF61-890305D32F4E}"/>
+    <hyperlink ref="J3" r:id="rId2" xr:uid="{23FF1BCF-BA21-4432-82E2-394717D6F28F}"/>
+    <hyperlink ref="J4" r:id="rId3" xr:uid="{5CCBC19C-AA8A-4B84-A094-BBE9093B7357}"/>
+    <hyperlink ref="J5" r:id="rId4" xr:uid="{B39DDC91-91FA-4D61-AD13-784D53C56D81}"/>
+    <hyperlink ref="J6" r:id="rId5" xr:uid="{75E22075-C933-438A-BB54-C8856AD36207}"/>
+    <hyperlink ref="J7" r:id="rId6" xr:uid="{88AD56B5-1488-4BDB-92F6-E8755F6D85B7}"/>
+    <hyperlink ref="J8" r:id="rId7" xr:uid="{F0045ED7-A666-46F9-A6A6-88C28E6AEAB7}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId8"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66F0071E-D3A6-4DED-AB23-7E39BD16B86A}">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:J1"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.2"/>
   <cols>
-    <col min="1" max="1" width="23.453125" customWidth="1"/>
-    <col min="2" max="2" width="14.1796875" customWidth="1"/>
-    <col min="3" max="3" width="23.36328125" customWidth="1"/>
-    <col min="4" max="4" width="21.453125" customWidth="1"/>
-    <col min="5" max="5" width="20.90625" customWidth="1"/>
-    <col min="6" max="6" width="18.1796875" customWidth="1"/>
-    <col min="7" max="7" width="19.54296875" customWidth="1"/>
-    <col min="8" max="8" width="18.81640625" customWidth="1"/>
-    <col min="9" max="9" width="19.36328125" customWidth="1"/>
-    <col min="10" max="10" width="19.7265625" customWidth="1"/>
+    <col min="1" max="1" width="23.44140625" customWidth="1"/>
+    <col min="2" max="2" width="14.21875" customWidth="1"/>
+    <col min="3" max="3" width="23.33203125" customWidth="1"/>
+    <col min="4" max="4" width="21.44140625" customWidth="1"/>
+    <col min="5" max="5" width="20.88671875" customWidth="1"/>
+    <col min="6" max="6" width="18.21875" customWidth="1"/>
+    <col min="7" max="7" width="19.5546875" customWidth="1"/>
+    <col min="8" max="8" width="18.77734375" customWidth="1"/>
+    <col min="9" max="9" width="19.33203125" customWidth="1"/>
+    <col min="10" max="10" width="19.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="62.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="31.8" thickBot="1">
       <c r="A1" s="3" t="s">
         <v>3</v>
       </c>
@@ -1064,8 +1465,141 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="13" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:10" ht="13.8" thickTop="1">
+      <c r="A2" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="E2" s="17">
+        <v>0.28599999999999998</v>
+      </c>
+      <c r="F2" t="s">
+        <v>71</v>
+      </c>
+      <c r="G2" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="H2" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="I2">
+        <v>1658878</v>
+      </c>
+      <c r="J2" s="18" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="E3" s="17">
+        <v>0.316</v>
+      </c>
+      <c r="F3" t="s">
+        <v>71</v>
+      </c>
+      <c r="G3" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="H3" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="I3">
+        <v>1833888</v>
+      </c>
+      <c r="J3" s="18" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="E4" s="17">
+        <v>0.28599999999999998</v>
+      </c>
+      <c r="F4" t="s">
+        <v>54</v>
+      </c>
+      <c r="G4" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="H4" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="I4">
+        <v>1577663</v>
+      </c>
+      <c r="J4" s="18" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="E5" s="17">
+        <v>7.89</v>
+      </c>
+      <c r="F5" t="s">
+        <v>85</v>
+      </c>
+      <c r="G5" t="s">
+        <v>79</v>
+      </c>
+      <c r="H5" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="I5">
+        <v>2356755</v>
+      </c>
+      <c r="J5" s="18" t="s">
+        <v>90</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="J2" r:id="rId1" xr:uid="{15CAB30B-1B17-4EA2-93EB-3AF073611C73}"/>
+    <hyperlink ref="J3" r:id="rId2" xr:uid="{4DCE092C-5662-456C-BCEA-F7C718E1C331}"/>
+    <hyperlink ref="J4" r:id="rId3" xr:uid="{71C13379-1621-463C-80E7-E45F800DC450}"/>
+    <hyperlink ref="J5" r:id="rId4" xr:uid="{70742694-AD27-44C8-940C-567047D26156}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>